<commit_message>
added try/except for openpyxl-max_row issue
</commit_message>
<xml_diff>
--- a/lists_for_chatterbird.xlsx
+++ b/lists_for_chatterbird.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\PycharmProjects\chatterbird_revised\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{854FB38A-BD3F-4185-ACF2-6DF8014B92CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715CE6F2-CC34-41ED-9043-65E645704D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{002EDD06-97FA-48C7-B006-6151D5A8012B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{002EDD06-97FA-48C7-B006-6151D5A8012B}"/>
   </bookViews>
   <sheets>
     <sheet name="управление" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="110">
   <si>
     <t>name</t>
   </si>
@@ -757,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE850D6F-0A85-4702-9865-92A31A3C9F96}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,6 +909,105 @@
         <v>28</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -918,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1274513-E87A-4F1D-80E9-9AD747EA09A4}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E2:E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>